<commit_message>
CSV de General Data acabados
</commit_message>
<xml_diff>
--- a/DesarrolloPy/DataSetOriginales/Bibliography_120220.xlsx
+++ b/DesarrolloPy/DataSetOriginales/Bibliography_120220.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\Universidad\PlataformaRefugiados\NAUTIA\DesarrolloPy\DataSetOriginales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F97F2D52-B19C-40D8-BCC8-899D7DF78957}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C905BE-9622-49B0-BBE3-5B17C076E819}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{CF48C59A-F23B-4BEB-B868-4FB1509D6440}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$C$49:$D$55</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="234">
   <si>
     <t>GENERAL INFORMATION - COUNTRY LEVEL</t>
   </si>
@@ -729,6 +732,12 @@
   </si>
   <si>
     <t>SETTLEMENTS Language 3</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>No</t>
   </si>
 </sst>
 </file>
@@ -1247,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBA903F-A3E6-4271-A750-242C97F6E0D6}">
   <dimension ref="A1:D192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A84" zoomScale="83" workbookViewId="0">
-      <selection activeCell="B94" sqref="B94"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="83" workbookViewId="0">
+      <selection activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -1882,7 +1891,9 @@
       <c r="B49" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="C49" s="6"/>
+      <c r="C49" s="6" t="s">
+        <v>233</v>
+      </c>
       <c r="D49" s="6"/>
     </row>
     <row r="50" spans="1:4">
@@ -1893,7 +1904,7 @@
         <v>85</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>86</v>
+        <v>232</v>
       </c>
       <c r="D50" s="6"/>
     </row>
@@ -1926,7 +1937,7 @@
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6" t="s">
-        <v>86</v>
+        <v>232</v>
       </c>
     </row>
     <row r="54" spans="1:4">
@@ -3547,6 +3558,11 @@
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Valores Validos de entrada: &quot;Si&quot; o &quot;No&quot;_x000a_Si es que no se puede dejar en blanco_x000a__x000a_" sqref="C49:D55" xr:uid="{BAF48672-73FD-4231-93D4-13AD26F429C3}">
+      <formula1>"Si, No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
arreglo de un tipo de datos en tabla camp, creacion de nuevos csv
</commit_message>
<xml_diff>
--- a/DesarrolloPy/DataSetOriginales/Bibliography_120220.xlsx
+++ b/DesarrolloPy/DataSetOriginales/Bibliography_120220.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\Universidad\PlataformaRefugiados\NAUTIA\DesarrolloPy\DataSetOriginales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5C905BE-9622-49B0-BBE3-5B17C076E819}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F90C28E2-229F-4463-8F7C-6084A5FA7DC2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{CF48C59A-F23B-4BEB-B868-4FB1509D6440}"/>
   </bookViews>
@@ -886,7 +886,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -896,6 +895,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1256,8 +1256,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBA903F-A3E6-4271-A750-242C97F6E0D6}">
   <dimension ref="A1:D192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="83" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView tabSelected="1" topLeftCell="A120" zoomScale="83" workbookViewId="0">
+      <selection activeCell="D129" sqref="D129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -1322,7 +1322,7 @@
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="24" t="s">
+      <c r="B5" s="23" t="s">
         <v>210</v>
       </c>
       <c r="C5" s="6">
@@ -1336,7 +1336,7 @@
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="24" t="s">
+      <c r="B6" s="23" t="s">
         <v>211</v>
       </c>
       <c r="C6" s="6">
@@ -1350,7 +1350,7 @@
       <c r="A7" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="24" t="s">
+      <c r="B7" s="23" t="s">
         <v>212</v>
       </c>
       <c r="C7" s="6">
@@ -1364,7 +1364,7 @@
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="24" t="s">
+      <c r="B8" s="23" t="s">
         <v>213</v>
       </c>
       <c r="C8" s="6">
@@ -1378,7 +1378,7 @@
       <c r="A9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="23" t="s">
         <v>214</v>
       </c>
       <c r="C9" s="6">
@@ -1392,7 +1392,7 @@
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="23" t="s">
         <v>215</v>
       </c>
       <c r="C10" s="6">
@@ -1406,7 +1406,7 @@
       <c r="A11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="24" t="s">
+      <c r="B11" s="23" t="s">
         <v>216</v>
       </c>
       <c r="C11" s="6">
@@ -1420,7 +1420,7 @@
       <c r="A12" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B12" s="24" t="s">
+      <c r="B12" s="23" t="s">
         <v>217</v>
       </c>
       <c r="C12" s="6">
@@ -2084,7 +2084,7 @@
       <c r="A66" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="B66" s="25" t="s">
+      <c r="B66" s="24" t="s">
         <v>218</v>
       </c>
       <c r="C66" s="6">
@@ -2098,7 +2098,7 @@
       <c r="A67" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="B67" s="25" t="s">
+      <c r="B67" s="24" t="s">
         <v>219</v>
       </c>
       <c r="C67" s="6">
@@ -2136,7 +2136,7 @@
       <c r="A70" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B70" s="25" t="s">
+      <c r="B70" s="24" t="s">
         <v>220</v>
       </c>
       <c r="C70" s="6">
@@ -2150,7 +2150,7 @@
       <c r="A71" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B71" s="25" t="s">
+      <c r="B71" s="24" t="s">
         <v>221</v>
       </c>
       <c r="C71" s="6">
@@ -2188,7 +2188,7 @@
       <c r="A74" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B74" s="25" t="s">
+      <c r="B74" s="24" t="s">
         <v>222</v>
       </c>
       <c r="C74" s="6">
@@ -2202,7 +2202,7 @@
       <c r="A75" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B75" s="25" t="s">
+      <c r="B75" s="24" t="s">
         <v>223</v>
       </c>
       <c r="C75" s="6">
@@ -2876,7 +2876,7 @@
       <c r="C129" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="D129" s="22">
+      <c r="D129" s="25">
         <v>33147</v>
       </c>
     </row>
@@ -2895,7 +2895,7 @@
       <c r="A131">
         <v>18.100000000000001</v>
       </c>
-      <c r="B131" s="23" t="s">
+      <c r="B131" s="22" t="s">
         <v>182</v>
       </c>
       <c r="C131" s="16" t="s">
@@ -2909,7 +2909,7 @@
       <c r="A132">
         <v>18.2</v>
       </c>
-      <c r="B132" s="23" t="s">
+      <c r="B132" s="22" t="s">
         <v>183</v>
       </c>
       <c r="C132" s="16" t="s">
@@ -2923,7 +2923,7 @@
       <c r="A133">
         <v>18.3</v>
       </c>
-      <c r="B133" s="23" t="s">
+      <c r="B133" s="22" t="s">
         <v>184</v>
       </c>
       <c r="C133" s="16" t="s">
@@ -2937,7 +2937,7 @@
       <c r="A134">
         <v>18.399999999999999</v>
       </c>
-      <c r="B134" s="23" t="s">
+      <c r="B134" s="22" t="s">
         <v>186</v>
       </c>
       <c r="C134" s="16" t="s">
@@ -2970,7 +2970,7 @@
       <c r="A137">
         <v>19.2</v>
       </c>
-      <c r="B137" s="23" t="s">
+      <c r="B137" s="22" t="s">
         <v>189</v>
       </c>
       <c r="C137" s="16" t="s">
@@ -2995,7 +2995,7 @@
       <c r="A139">
         <v>19.399999999999999</v>
       </c>
-      <c r="B139" s="23" t="s">
+      <c r="B139" s="22" t="s">
         <v>191</v>
       </c>
       <c r="C139" s="16" t="s">
@@ -3017,7 +3017,7 @@
       <c r="A141">
         <v>20.100000000000001</v>
       </c>
-      <c r="B141" s="23" t="s">
+      <c r="B141" s="22" t="s">
         <v>193</v>
       </c>
       <c r="C141" s="16" t="s">
@@ -3031,7 +3031,7 @@
       <c r="A142">
         <v>20.2</v>
       </c>
-      <c r="B142" s="23" t="s">
+      <c r="B142" s="22" t="s">
         <v>194</v>
       </c>
       <c r="C142" s="16" t="s">
@@ -3045,7 +3045,7 @@
       <c r="A143">
         <v>20.3</v>
       </c>
-      <c r="B143" s="23" t="s">
+      <c r="B143" s="22" t="s">
         <v>195</v>
       </c>
       <c r="C143" s="16" t="s">
@@ -3084,7 +3084,7 @@
       <c r="A146">
         <v>22.1</v>
       </c>
-      <c r="B146" s="23" t="s">
+      <c r="B146" s="22" t="s">
         <v>198</v>
       </c>
       <c r="C146" s="16" t="s">
@@ -3098,7 +3098,7 @@
       <c r="A147">
         <v>22.2</v>
       </c>
-      <c r="B147" s="23" t="s">
+      <c r="B147" s="22" t="s">
         <v>199</v>
       </c>
       <c r="C147" s="16" t="s">
@@ -3558,11 +3558,16 @@
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Valores Validos de entrada: &quot;Si&quot; o &quot;No&quot;_x000a_Si es que no se puede dejar en blanco_x000a__x000a_" sqref="C49:D55" xr:uid="{BAF48672-73FD-4231-93D4-13AD26F429C3}">
       <formula1>"Si, No"</formula1>
     </dataValidation>
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Formato fecha" prompt="DD/MM/AAAA" sqref="D129" xr:uid="{0CC26212-6430-410E-8979-27DFBA36E156}">
+      <formula1>36526</formula1>
+      <formula2>402133</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Refactorización de la tabla Camp en BBDD y continuación con script ETL'
</commit_message>
<xml_diff>
--- a/DesarrolloPy/DataSetOriginales/Bibliography_120220.xlsx
+++ b/DesarrolloPy/DataSetOriginales/Bibliography_120220.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\Universidad\PlataformaRefugiados\NAUTIA\DesarrolloPy\DataSetOriginales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{211F7519-828D-40F1-9A11-46BCD8F11202}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45B40F7-C65E-48A5-89B1-6F6D4032EE05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{CF48C59A-F23B-4BEB-B868-4FB1509D6440}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="211">
   <si>
     <t>GENERAL INFORMATION - COUNTRY LEVEL</t>
   </si>
@@ -666,6 +666,9 @@
   </si>
   <si>
     <t>SETTLEMENTS Language 3</t>
+  </si>
+  <si>
+    <t>Af</t>
   </si>
 </sst>
 </file>
@@ -1184,8 +1187,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBA903F-A3E6-4271-A750-242C97F6E0D6}">
   <dimension ref="A1:D192"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="83" workbookViewId="0">
-      <selection activeCell="D54" sqref="D54"/>
+    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="83" workbookViewId="0">
+      <selection activeCell="F137" sqref="F137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -2557,6 +2560,9 @@
         <v>166</v>
       </c>
       <c r="C136" s="16"/>
+      <c r="D136" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137">

</xml_diff>

<commit_message>
cambios en modelos sql y en bibliografia. Resto avance normal
</commit_message>
<xml_diff>
--- a/DesarrolloPy/DataSetOriginales/Bibliography_120220.xlsx
+++ b/DesarrolloPy/DataSetOriginales/Bibliography_120220.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\Universidad\PlataformaRefugiados\NAUTIA\DesarrolloPy\DataSetOriginales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09842E5B-2DB7-47B3-8EDF-8F4E03A64FA5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C833373-0DAD-40F0-83CC-9D2BC19CEE85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{CF48C59A-F23B-4BEB-B868-4FB1509D6440}"/>
   </bookViews>
@@ -1298,8 +1298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBA903F-A3E6-4271-A750-242C97F6E0D6}">
   <dimension ref="A1:D192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" zoomScale="92" workbookViewId="0">
-      <selection activeCell="E163" sqref="E163"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="92" workbookViewId="0">
+      <selection activeCell="D118" sqref="D118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -3166,7 +3166,7 @@
     <cfRule type="duplicateValues" dxfId="1" priority="2"/>
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <dataValidations count="6">
+  <dataValidations count="7">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Valores Validos de entrada: &quot;Si&quot; o &quot;No&quot;_x000a_Si es que no se puede dejar en blanco_x000a__x000a_" sqref="C49:D55" xr:uid="{BAF48672-73FD-4231-93D4-13AD26F429C3}">
       <formula1>"Si, No"</formula1>
     </dataValidation>
@@ -3186,6 +3186,9 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D139" xr:uid="{5D300C50-C4CF-46DD-B628-47DF481CEA31}">
       <formula1>"Dfa,Bwa,Dsa,Dfb,Dwb,Dsb"</formula1>
     </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C115:D118" xr:uid="{11A8FA3E-F4F7-43D9-84D4-67EC08F949B6}">
+      <formula1>"yes,no"</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
avance normal con rectificaciones en modelo sql
</commit_message>
<xml_diff>
--- a/DesarrolloPy/DataSetOriginales/Bibliography_120220.xlsx
+++ b/DesarrolloPy/DataSetOriginales/Bibliography_120220.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\Universidad\PlataformaRefugiados\NAUTIA\DesarrolloPy\DataSetOriginales\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C833373-0DAD-40F0-83CC-9D2BC19CEE85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A11157-E1AF-4D32-9012-D7E4D20B210B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{CF48C59A-F23B-4BEB-B868-4FB1509D6440}"/>
   </bookViews>
@@ -470,9 +470,6 @@
     <t>Cause 3</t>
   </si>
   <si>
-    <t xml:space="preserve">Affected groups due to food insecurity </t>
-  </si>
-  <si>
     <t>Children</t>
   </si>
   <si>
@@ -774,6 +771,9 @@
   </si>
   <si>
     <t>ld.6</t>
+  </si>
+  <si>
+    <t>Affected groups due to food insecurity</t>
   </si>
 </sst>
 </file>
@@ -1299,7 +1299,7 @@
   <dimension ref="A1:D192"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A103" zoomScale="92" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+      <selection activeCell="B114" sqref="B114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -1357,7 +1357,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
@@ -1367,7 +1367,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -1377,7 +1377,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1387,7 +1387,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -1397,7 +1397,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -1407,7 +1407,7 @@
         <v>11</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -1417,7 +1417,7 @@
         <v>12</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -1427,7 +1427,7 @@
         <v>13</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
@@ -1971,7 +1971,7 @@
         <v>96</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C66" s="6"/>
       <c r="D66" s="3"/>
@@ -1981,7 +1981,7 @@
         <v>97</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C67" s="6"/>
       <c r="D67" s="3"/>
@@ -2011,7 +2011,7 @@
         <v>100</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C70" s="6"/>
       <c r="D70" s="3"/>
@@ -2021,7 +2021,7 @@
         <v>101</v>
       </c>
       <c r="B71" s="24" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C71" s="6"/>
       <c r="D71" s="3"/>
@@ -2051,7 +2051,7 @@
         <v>104</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C74" s="6"/>
       <c r="D74" s="3"/>
@@ -2061,7 +2061,7 @@
         <v>105</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C75" s="6"/>
       <c r="D75" s="3"/>
@@ -2251,7 +2251,7 @@
         <v>9</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2259,7 +2259,7 @@
         <v>9.1</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C95" s="9"/>
       <c r="D95" s="10"/>
@@ -2269,7 +2269,7 @@
         <v>9.1999999999999993</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C96" s="9"/>
       <c r="D96" s="10"/>
@@ -2279,7 +2279,7 @@
         <v>9.3000000000000007</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C97" s="9"/>
       <c r="D97" s="10"/>
@@ -2289,7 +2289,7 @@
         <v>10</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2297,7 +2297,7 @@
         <v>10.1</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C99" s="9"/>
       <c r="D99" s="10"/>
@@ -2307,7 +2307,7 @@
         <v>10.199999999999999</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C100" s="9"/>
       <c r="D100" s="10"/>
@@ -2317,7 +2317,7 @@
         <v>10.3</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C101" s="9"/>
       <c r="D101" s="10"/>
@@ -2433,7 +2433,7 @@
         <v>14</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>144</v>
+        <v>245</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2441,7 +2441,7 @@
         <v>14.1</v>
       </c>
       <c r="B115" s="16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="116" spans="1:4">
@@ -2449,7 +2449,7 @@
         <v>14.2</v>
       </c>
       <c r="B116" s="16" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="117" spans="1:4">
@@ -2457,7 +2457,7 @@
         <v>14.3</v>
       </c>
       <c r="B117" s="16" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2465,7 +2465,7 @@
         <v>14.4</v>
       </c>
       <c r="B118" s="16" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2473,7 +2473,7 @@
         <v>15</v>
       </c>
       <c r="B119" s="17" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="120" spans="1:4">
@@ -2481,7 +2481,7 @@
         <v>15.1</v>
       </c>
       <c r="B120" s="16" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C120">
         <v>2</v>
@@ -2495,7 +2495,7 @@
         <v>15.2</v>
       </c>
       <c r="B121" s="18" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C121">
         <v>1.8</v>
@@ -2509,7 +2509,7 @@
         <v>15.3</v>
       </c>
       <c r="B122" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C122">
         <v>1.3</v>
@@ -2523,7 +2523,7 @@
         <v>15.4</v>
       </c>
       <c r="B123" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C123">
         <v>1.25</v>
@@ -2537,7 +2537,7 @@
         <v>15.5</v>
       </c>
       <c r="B124" s="18" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C124">
         <v>3.5</v>
@@ -2551,7 +2551,7 @@
         <v>15.6</v>
       </c>
       <c r="B125" s="18" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C125">
         <v>3.5</v>
@@ -2565,7 +2565,7 @@
         <v>15.7</v>
       </c>
       <c r="B126" s="18" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C126">
         <v>2</v>
@@ -2579,7 +2579,7 @@
         <v>16</v>
       </c>
       <c r="B127" s="20" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C127">
         <v>70</v>
@@ -2590,7 +2590,7 @@
     </row>
     <row r="128" spans="1:4">
       <c r="B128" s="21" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C128" s="5" t="s">
         <v>131</v>
@@ -2604,7 +2604,7 @@
         <v>17</v>
       </c>
       <c r="B129" s="14" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C129" s="16"/>
       <c r="D129" s="25"/>
@@ -2614,7 +2614,7 @@
         <v>18</v>
       </c>
       <c r="B130" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C130" s="16"/>
     </row>
@@ -2623,7 +2623,7 @@
         <v>18.100000000000001</v>
       </c>
       <c r="B131" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C131" s="16"/>
     </row>
@@ -2632,7 +2632,7 @@
         <v>18.2</v>
       </c>
       <c r="B132" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C132" s="16"/>
     </row>
@@ -2641,7 +2641,7 @@
         <v>18.3</v>
       </c>
       <c r="B133" s="22" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C133" s="16"/>
     </row>
@@ -2650,7 +2650,7 @@
         <v>18.399999999999999</v>
       </c>
       <c r="B134" s="22" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C134" s="16"/>
     </row>
@@ -2659,7 +2659,7 @@
         <v>19</v>
       </c>
       <c r="B135" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C135" s="16"/>
     </row>
@@ -2668,11 +2668,11 @@
         <v>19.100000000000001</v>
       </c>
       <c r="B136" s="16" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C136" s="16"/>
       <c r="D136" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2680,7 +2680,7 @@
         <v>19.2</v>
       </c>
       <c r="B137" s="22" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C137" s="16"/>
     </row>
@@ -2689,7 +2689,7 @@
         <v>19.3</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C138" s="16"/>
     </row>
@@ -2698,7 +2698,7 @@
         <v>19.399999999999999</v>
       </c>
       <c r="B139" s="22" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C139" s="16"/>
     </row>
@@ -2707,7 +2707,7 @@
         <v>20</v>
       </c>
       <c r="B140" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C140" s="16"/>
     </row>
@@ -2716,7 +2716,7 @@
         <v>20.100000000000001</v>
       </c>
       <c r="B141" s="22" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C141" s="16"/>
     </row>
@@ -2725,7 +2725,7 @@
         <v>20.2</v>
       </c>
       <c r="B142" s="22" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C142" s="16"/>
     </row>
@@ -2734,7 +2734,7 @@
         <v>20.3</v>
       </c>
       <c r="B143" s="22" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C143" s="16"/>
     </row>
@@ -2743,7 +2743,7 @@
         <v>21</v>
       </c>
       <c r="B144" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C144" s="16"/>
     </row>
@@ -2752,7 +2752,7 @@
         <v>22</v>
       </c>
       <c r="B145" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C145" s="16"/>
     </row>
@@ -2761,7 +2761,7 @@
         <v>22.1</v>
       </c>
       <c r="B146" s="22" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C146" s="16"/>
     </row>
@@ -2770,7 +2770,7 @@
         <v>22.2</v>
       </c>
       <c r="B147" s="22" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C147" s="16"/>
     </row>
@@ -2779,7 +2779,7 @@
         <v>23</v>
       </c>
       <c r="B148" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C148" s="16"/>
     </row>
@@ -2788,7 +2788,7 @@
         <v>24</v>
       </c>
       <c r="B149" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C149" s="16"/>
     </row>
@@ -2797,7 +2797,7 @@
         <v>25</v>
       </c>
       <c r="B150" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C150" s="16"/>
     </row>
@@ -2806,7 +2806,7 @@
         <v>26</v>
       </c>
       <c r="B151" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C151" s="16"/>
     </row>
@@ -2815,7 +2815,7 @@
         <v>26.1</v>
       </c>
       <c r="B152" s="22" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C152" s="16"/>
     </row>
@@ -2824,7 +2824,7 @@
         <v>26.2</v>
       </c>
       <c r="B153" s="22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C153" s="16"/>
     </row>
@@ -2833,7 +2833,7 @@
         <v>26.3</v>
       </c>
       <c r="B154" s="22" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C154" s="16"/>
     </row>
@@ -2842,13 +2842,13 @@
         <v>26.4</v>
       </c>
       <c r="B155" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C155" s="16"/>
     </row>
     <row r="156" spans="1:4">
       <c r="B156" s="2" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C156" s="5" t="s">
         <v>131</v>
@@ -2862,7 +2862,7 @@
         <v>27</v>
       </c>
       <c r="B157" s="15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2870,7 +2870,7 @@
         <v>27.1</v>
       </c>
       <c r="B158" s="22" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C158" s="16"/>
     </row>
@@ -2879,7 +2879,7 @@
         <v>27.2</v>
       </c>
       <c r="B159" s="22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2887,7 +2887,7 @@
         <v>27.3</v>
       </c>
       <c r="B160" s="22" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="161" spans="1:3">
@@ -2895,7 +2895,7 @@
         <v>27.4</v>
       </c>
       <c r="B161" s="22" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="162" spans="1:3">
@@ -2903,7 +2903,7 @@
         <v>27.5</v>
       </c>
       <c r="B162" s="22" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="163" spans="1:3">
@@ -2911,7 +2911,7 @@
         <v>27.6</v>
       </c>
       <c r="B163" s="22" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="164" spans="1:3">
@@ -2919,7 +2919,7 @@
         <v>27.7</v>
       </c>
       <c r="B164" s="22" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="165" spans="1:3">
@@ -2927,7 +2927,7 @@
         <v>28</v>
       </c>
       <c r="B165" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="166" spans="1:3">
@@ -2935,7 +2935,7 @@
         <v>28.1</v>
       </c>
       <c r="B166" s="22" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C166" s="16"/>
     </row>
@@ -2944,7 +2944,7 @@
         <v>28.2</v>
       </c>
       <c r="B167" s="22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="168" spans="1:3">
@@ -2952,7 +2952,7 @@
         <v>28.3</v>
       </c>
       <c r="B168" s="22" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="169" spans="1:3">
@@ -2960,7 +2960,7 @@
         <v>28.4</v>
       </c>
       <c r="B169" s="22" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="170" spans="1:3">
@@ -2968,7 +2968,7 @@
         <v>28.5</v>
       </c>
       <c r="B170" s="22" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="171" spans="1:3">
@@ -2976,7 +2976,7 @@
         <v>28.6</v>
       </c>
       <c r="B171" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="172" spans="1:3">
@@ -2984,7 +2984,7 @@
         <v>29</v>
       </c>
       <c r="B172" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="173" spans="1:3">
@@ -2992,7 +2992,7 @@
         <v>29.1</v>
       </c>
       <c r="B173" s="22" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C173" s="16"/>
     </row>
@@ -3001,7 +3001,7 @@
         <v>29.2</v>
       </c>
       <c r="B174" s="22" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="175" spans="1:3">
@@ -3009,7 +3009,7 @@
         <v>29.3</v>
       </c>
       <c r="B175" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="176" spans="1:3">
@@ -3017,7 +3017,7 @@
         <v>29.4</v>
       </c>
       <c r="B176" s="22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="177" spans="1:3">
@@ -3025,7 +3025,7 @@
         <v>29.5</v>
       </c>
       <c r="B177" s="22" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="178" spans="1:3">
@@ -3033,7 +3033,7 @@
         <v>29.6</v>
       </c>
       <c r="B178" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="179" spans="1:3">
@@ -3041,7 +3041,7 @@
         <v>30</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="180" spans="1:3">
@@ -3049,7 +3049,7 @@
         <v>30.1</v>
       </c>
       <c r="B180" s="16" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C180" s="16"/>
     </row>
@@ -3058,7 +3058,7 @@
         <v>30.2</v>
       </c>
       <c r="B181" s="16" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="182" spans="1:3">
@@ -3066,7 +3066,7 @@
         <v>30.3</v>
       </c>
       <c r="B182" s="16" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="183" spans="1:3">
@@ -3074,7 +3074,7 @@
         <v>30.4</v>
       </c>
       <c r="B183" s="16" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="184" spans="1:3">
@@ -3082,7 +3082,7 @@
         <v>30.5</v>
       </c>
       <c r="B184" s="16" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="185" spans="1:3">
@@ -3090,7 +3090,7 @@
         <v>30.6</v>
       </c>
       <c r="B185" s="16" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="186" spans="1:3">
@@ -3098,7 +3098,7 @@
         <v>31</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="187" spans="1:3">
@@ -3106,7 +3106,7 @@
         <v>31.1</v>
       </c>
       <c r="B187" s="16" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C187" s="16"/>
     </row>
@@ -3115,7 +3115,7 @@
         <v>31.2</v>
       </c>
       <c r="B188" s="16" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="189" spans="1:3">
@@ -3123,7 +3123,7 @@
         <v>31.3</v>
       </c>
       <c r="B189" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="190" spans="1:3">
@@ -3131,7 +3131,7 @@
         <v>31.4</v>
       </c>
       <c r="B190" s="16" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="191" spans="1:3">
@@ -3139,7 +3139,7 @@
         <v>31.5</v>
       </c>
       <c r="B191" s="16" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="192" spans="1:3">
@@ -3147,7 +3147,7 @@
         <v>31.6</v>
       </c>
       <c r="B192" s="16" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Perfeccionamiento de CreateLoadDataInfle incluyendo las columnas de cada tabla
</commit_message>
<xml_diff>
--- a/DesarrolloPy/DataSetOriginales/Bibliography_120220.xlsx
+++ b/DesarrolloPy/DataSetOriginales/Bibliography_120220.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guill\Documents\Universidad\PlataformaRefugiados\NAUTIA\DesarrolloPy\DataSetOriginales\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\formularios odk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A11157-E1AF-4D32-9012-D7E4D20B210B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{CF48C59A-F23B-4BEB-B868-4FB1509D6440}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,25 +17,17 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$C$49:$D$55</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="298">
   <si>
     <t>GENERAL INFORMATION - COUNTRY LEVEL</t>
   </si>
@@ -569,12 +560,6 @@
     <t>Min (mm)</t>
   </si>
   <si>
-    <t>Solar irradiance (kW/m2/day)</t>
-  </si>
-  <si>
-    <t>Wind speed</t>
-  </si>
-  <si>
     <t>Additional information</t>
   </si>
   <si>
@@ -665,9 +650,6 @@
     <t>SETTLEMENTS Language 3</t>
   </si>
   <si>
-    <t>Af</t>
-  </si>
-  <si>
     <t>r.1</t>
   </si>
   <si>
@@ -774,13 +756,178 @@
   </si>
   <si>
     <t>Affected groups due to food insecurity</t>
+  </si>
+  <si>
+    <t>Etiopia</t>
+  </si>
+  <si>
+    <t>Eritrea</t>
+  </si>
+  <si>
+    <t>Oromo</t>
+  </si>
+  <si>
+    <t>Amara</t>
+  </si>
+  <si>
+    <t>Tiigray</t>
+  </si>
+  <si>
+    <t>Kunama</t>
+  </si>
+  <si>
+    <t>Triginya</t>
+  </si>
+  <si>
+    <t>Saho</t>
+  </si>
+  <si>
+    <t>Islam</t>
+  </si>
+  <si>
+    <t>Cristianismo Ortodoxo</t>
+  </si>
+  <si>
+    <t>Protestantismo</t>
+  </si>
+  <si>
+    <t>Cristianismo</t>
+  </si>
+  <si>
+    <t>iIslam</t>
+  </si>
+  <si>
+    <t>Trigrinya</t>
+  </si>
+  <si>
+    <t>Tigrinya</t>
+  </si>
+  <si>
+    <t>Birr</t>
+  </si>
+  <si>
+    <t>Nakfa</t>
+  </si>
+  <si>
+    <t>1ERN = 0,065 USD</t>
+  </si>
+  <si>
+    <t>1 ETB = 0,0363915 USD</t>
+  </si>
+  <si>
+    <t>Si</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">residential &gt; 500 kWh = 0.6943 birr + service cost </t>
+  </si>
+  <si>
+    <t>Árabe</t>
+  </si>
+  <si>
+    <t>poor quality of food</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> droughts </t>
+  </si>
+  <si>
+    <t>food scarcity</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Administration for Refugee and Returnee Affairs (ARRA)</t>
+  </si>
+  <si>
+    <t>National Resource Development and Environmental Protection Office (NRDEP)</t>
+  </si>
+  <si>
+    <t>Ethiopian Electric Utility</t>
+  </si>
+  <si>
+    <t>United Nations High Commissioner for Refugees (UNHCR)</t>
+  </si>
+  <si>
+    <t>World Food Program (WFP)</t>
+  </si>
+  <si>
+    <t>United Nations Childrens Fund (UNICEF)</t>
+  </si>
+  <si>
+    <t>International Organization for Migration (IOM)</t>
+  </si>
+  <si>
+    <t>International Committee of RED Cross (ICRC)</t>
+  </si>
+  <si>
+    <t>Ethiopian Orthodox Church, Development and Inter-Church Aid Department (EOC/DICAD)</t>
+  </si>
+  <si>
+    <t>Opportunities Industrialization Centre - Ethiopia (OICE)</t>
+  </si>
+  <si>
+    <t>International Rescue Committee (IRC)</t>
+  </si>
+  <si>
+    <t>Norwegian Refugee Council (NRC)</t>
+  </si>
+  <si>
+    <t>Jesuit Refugee Service (JRS)</t>
+  </si>
+  <si>
+    <t>Centre of Victims of Torture (CVT)</t>
+  </si>
+  <si>
+    <t>Medecins Sans Frontieres (MSF-H)</t>
+  </si>
+  <si>
+    <t>Innovative Humanitarian Solutions (IHS</t>
+  </si>
+  <si>
+    <t>Asociación Española de Cooperación Internacional para el Desarrollo (AECID)</t>
+  </si>
+  <si>
+    <t>IBERDROLA S.A.</t>
+  </si>
+  <si>
+    <t>Fundación ACCIONA Microenergía</t>
+  </si>
+  <si>
+    <t>itdUPM</t>
+  </si>
+  <si>
+    <t>Philips</t>
+  </si>
+  <si>
+    <t>Aw</t>
+  </si>
+  <si>
+    <t>war</t>
+  </si>
+  <si>
+    <t>poor</t>
+  </si>
+  <si>
+    <t>politic persecution</t>
+  </si>
+  <si>
+    <t>Wind speed km/h</t>
+  </si>
+  <si>
+    <t>Solar irradiance (kW/h)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -848,6 +995,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF505050"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -879,7 +1032,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -938,12 +1091,29 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1" xr:uid="{5261E692-EA18-4C66-80B0-A3C156F09071}"/>
+    <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="4">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -959,16 +1129,6 @@
           <color rgb="FF9C0006"/>
         </bottom>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1295,19 +1455,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BBA903F-A3E6-4271-A750-242C97F6E0D6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="92" workbookViewId="0">
-      <selection activeCell="B114" sqref="B114"/>
+    <sheetView tabSelected="1" topLeftCell="A149" zoomScale="92" workbookViewId="0">
+      <selection activeCell="N190" sqref="N189:N190"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="4.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.36328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1339,8 +1499,12 @@
       <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
+      <c r="C3" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="1">
@@ -1357,80 +1521,112 @@
         <v>6</v>
       </c>
       <c r="B5" s="23" t="s">
-        <v>187</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
+        <v>185</v>
+      </c>
+      <c r="C5" s="6">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6">
+        <v>12</v>
+      </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="23" t="s">
-        <v>188</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
+        <v>186</v>
+      </c>
+      <c r="C6" s="6">
+        <v>12</v>
+      </c>
+      <c r="D6" s="6">
+        <v>8</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="23" t="s">
-        <v>189</v>
-      </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
+        <v>187</v>
+      </c>
+      <c r="C7" s="6">
+        <v>15</v>
+      </c>
+      <c r="D7" s="6">
+        <v>10</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="23" t="s">
-        <v>190</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
+        <v>188</v>
+      </c>
+      <c r="C8" s="6">
+        <v>25</v>
+      </c>
+      <c r="D8" s="6">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="23" t="s">
-        <v>191</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
+        <v>189</v>
+      </c>
+      <c r="C9" s="6">
+        <v>20</v>
+      </c>
+      <c r="D9" s="6">
+        <v>25</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B10" s="23" t="s">
-        <v>192</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
+        <v>190</v>
+      </c>
+      <c r="C10" s="6">
+        <v>10</v>
+      </c>
+      <c r="D10" s="6">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>193</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
+        <v>191</v>
+      </c>
+      <c r="C11" s="6">
+        <v>6</v>
+      </c>
+      <c r="D11" s="6">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="23" t="s">
-        <v>194</v>
-      </c>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
+        <v>192</v>
+      </c>
+      <c r="C12" s="6">
+        <v>4</v>
+      </c>
+      <c r="D12" s="6">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="1">
@@ -1449,8 +1645,12 @@
       <c r="B14" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="6"/>
+      <c r="C14" s="6">
+        <v>20</v>
+      </c>
+      <c r="D14" s="6">
+        <v>10</v>
+      </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
@@ -1459,8 +1659,12 @@
       <c r="B15" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
+      <c r="C15" s="6">
+        <v>40</v>
+      </c>
+      <c r="D15" s="6">
+        <v>25</v>
+      </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="3" t="s">
@@ -1469,8 +1673,12 @@
       <c r="B16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="6"/>
-      <c r="D16" s="6"/>
+      <c r="C16" s="6">
+        <v>30</v>
+      </c>
+      <c r="D16" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="3" t="s">
@@ -1479,8 +1687,12 @@
       <c r="B17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="C17" s="6">
+        <v>10</v>
+      </c>
+      <c r="D17" s="6">
+        <v>25</v>
+      </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1">
@@ -1489,8 +1701,12 @@
       <c r="B18" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
+      <c r="C18" s="6">
+        <v>2.85</v>
+      </c>
+      <c r="D18" s="6">
+        <v>1.9</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="1">
@@ -1499,8 +1715,12 @@
       <c r="B19" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
+      <c r="C19" s="6">
+        <v>0.86</v>
+      </c>
+      <c r="D19" s="6">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="1">
@@ -1509,8 +1729,12 @@
       <c r="B20" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C20" s="6"/>
-      <c r="D20" s="6"/>
+      <c r="C20" s="6">
+        <v>0.44800000000000001</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.40200000000000002</v>
+      </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="1">
@@ -1519,8 +1743,12 @@
       <c r="B21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="6"/>
-      <c r="D21" s="6"/>
+      <c r="C21" s="6">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="D21" s="6">
+        <v>64.2</v>
+      </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="2">
@@ -1549,8 +1777,12 @@
       <c r="B24" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="9"/>
-      <c r="D24" s="6"/>
+      <c r="C24" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="D24" s="10" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="3" t="s">
@@ -1559,8 +1791,12 @@
       <c r="B25" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="9"/>
-      <c r="D25" s="6"/>
+      <c r="C25" s="10" t="s">
+        <v>246</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="3" t="s">
@@ -1569,8 +1805,12 @@
       <c r="B26" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C26" s="9"/>
-      <c r="D26" s="6"/>
+      <c r="C26" s="10" t="s">
+        <v>247</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="1">
@@ -1589,8 +1829,12 @@
       <c r="B28" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="9"/>
-      <c r="D28" s="10"/>
+      <c r="C28" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D28" s="10" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="3" t="s">
@@ -1599,8 +1843,12 @@
       <c r="B29" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C29" s="9"/>
-      <c r="D29" s="10"/>
+      <c r="C29" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="D29" s="10" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="3" t="s">
@@ -1609,7 +1857,9 @@
       <c r="B30" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C30" s="9"/>
+      <c r="C30" s="10" t="s">
+        <v>253</v>
+      </c>
       <c r="D30" s="10"/>
     </row>
     <row r="31" spans="1:4">
@@ -1629,8 +1879,12 @@
       <c r="B32" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="10"/>
+      <c r="C32" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="3" t="s">
@@ -1639,8 +1893,12 @@
       <c r="B33" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C33" s="9"/>
-      <c r="D33" s="10"/>
+      <c r="C33" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="D33" s="10" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="3" t="s">
@@ -1649,7 +1907,7 @@
       <c r="B34" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="9"/>
+      <c r="C34" s="10"/>
       <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:4">
@@ -1669,7 +1927,9 @@
       <c r="B36" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C36" s="6"/>
+      <c r="C36" s="6">
+        <v>79.41</v>
+      </c>
       <c r="D36" s="6"/>
     </row>
     <row r="37" spans="1:4">
@@ -1679,8 +1939,12 @@
       <c r="B37" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
+      <c r="C37" s="6">
+        <v>40</v>
+      </c>
+      <c r="D37" s="6">
+        <v>20</v>
+      </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="3" t="s">
@@ -1689,8 +1953,12 @@
       <c r="B38" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
+      <c r="C38" s="6">
+        <v>35</v>
+      </c>
+      <c r="D38" s="6">
+        <v>10</v>
+      </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="3" t="s">
@@ -1699,8 +1967,12 @@
       <c r="B39" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
+      <c r="C39" s="6">
+        <v>5</v>
+      </c>
+      <c r="D39" s="6">
+        <v>30</v>
+      </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="3" t="s">
@@ -1709,8 +1981,12 @@
       <c r="B40" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
+      <c r="C40" s="6">
+        <v>20</v>
+      </c>
+      <c r="D40" s="6">
+        <v>40</v>
+      </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="1">
@@ -1719,8 +1995,12 @@
       <c r="B41" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="10"/>
+      <c r="C41" s="6">
+        <v>23.5</v>
+      </c>
+      <c r="D41" s="10">
+        <v>53</v>
+      </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="1">
@@ -1729,7 +2009,9 @@
       <c r="B42" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="C42" s="6"/>
+      <c r="C42" s="6">
+        <v>39.1</v>
+      </c>
       <c r="D42" s="10"/>
     </row>
     <row r="43" spans="1:4">
@@ -1739,8 +2021,12 @@
       <c r="B43" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C43" s="6"/>
-      <c r="D43" s="10"/>
+      <c r="C43" s="6">
+        <v>767</v>
+      </c>
+      <c r="D43" s="10">
+        <v>236</v>
+      </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="1">
@@ -1763,8 +2049,12 @@
       <c r="B45" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
+      <c r="C45" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>259</v>
+      </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="1">
@@ -1773,8 +2063,12 @@
       <c r="B46" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
+      <c r="C46" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="2">
@@ -1803,8 +2097,12 @@
       <c r="B49" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
+      <c r="C49" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="3" t="s">
@@ -1813,8 +2111,12 @@
       <c r="B50" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
+      <c r="C50" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>262</v>
+      </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="3" t="s">
@@ -1823,8 +2125,12 @@
       <c r="B51" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
+      <c r="C51" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D51" s="6" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="3" t="s">
@@ -1833,8 +2139,12 @@
       <c r="B52" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
+      <c r="C52" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="3" t="s">
@@ -1843,8 +2153,12 @@
       <c r="B53" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
+      <c r="C53" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="3" t="s">
@@ -1853,8 +2167,12 @@
       <c r="B54" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
+      <c r="C54" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D54" s="6" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="3" t="s">
@@ -1863,8 +2181,12 @@
       <c r="B55" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
+      <c r="C55" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="D55" s="6" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="56" spans="1:4">
       <c r="A56" s="2">
@@ -1893,8 +2215,12 @@
       <c r="B58" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="C58" s="6"/>
-      <c r="D58" s="3"/>
+      <c r="C58" s="6">
+        <v>20.7</v>
+      </c>
+      <c r="D58" s="3">
+        <v>35.770000000000003</v>
+      </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59" s="3" t="s">
@@ -1903,8 +2229,12 @@
       <c r="B59" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="C59" s="6"/>
-      <c r="D59" s="3"/>
+      <c r="C59" s="6">
+        <v>79.3</v>
+      </c>
+      <c r="D59" s="3">
+        <v>64.23</v>
+      </c>
     </row>
     <row r="60" spans="1:4">
       <c r="A60" s="1">
@@ -1923,8 +2253,12 @@
       <c r="B61" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="C61" s="6"/>
-      <c r="D61" s="3"/>
+      <c r="C61" s="6">
+        <v>7000</v>
+      </c>
+      <c r="D61" s="3">
+        <v>3000</v>
+      </c>
     </row>
     <row r="62" spans="1:4">
       <c r="A62" s="3" t="s">
@@ -1933,8 +2267,12 @@
       <c r="B62" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="C62" s="6"/>
-      <c r="D62" s="3"/>
+      <c r="C62" s="6">
+        <v>2900</v>
+      </c>
+      <c r="D62" s="3">
+        <v>1200</v>
+      </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63" s="1">
@@ -1964,16 +2302,20 @@
         <v>95</v>
       </c>
       <c r="C65" s="6"/>
-      <c r="D65" s="3"/>
+      <c r="D65" s="3">
+        <v>47</v>
+      </c>
     </row>
     <row r="66" spans="1:4">
       <c r="A66" s="3" t="s">
         <v>96</v>
       </c>
       <c r="B66" s="24" t="s">
-        <v>195</v>
-      </c>
-      <c r="C66" s="6"/>
+        <v>193</v>
+      </c>
+      <c r="C66" s="6">
+        <v>66</v>
+      </c>
       <c r="D66" s="3"/>
     </row>
     <row r="67" spans="1:4">
@@ -1981,9 +2323,11 @@
         <v>97</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>196</v>
-      </c>
-      <c r="C67" s="6"/>
+        <v>194</v>
+      </c>
+      <c r="C67" s="6">
+        <v>95</v>
+      </c>
       <c r="D67" s="3"/>
     </row>
     <row r="68" spans="1:4">
@@ -2004,24 +2348,28 @@
         <v>95</v>
       </c>
       <c r="C69" s="6"/>
-      <c r="D69" s="3"/>
+      <c r="D69" s="3">
+        <v>16</v>
+      </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70" s="3" t="s">
         <v>100</v>
       </c>
       <c r="B70" s="24" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C70" s="6"/>
-      <c r="D70" s="3"/>
+      <c r="D70" s="3">
+        <v>30</v>
+      </c>
     </row>
     <row r="71" spans="1:4">
       <c r="A71" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B71" s="24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C71" s="6"/>
       <c r="D71" s="3"/>
@@ -2043,28 +2391,40 @@
       <c r="B73" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="C73" s="6"/>
-      <c r="D73" s="3"/>
+      <c r="C73" s="6">
+        <v>57</v>
+      </c>
+      <c r="D73" s="3">
+        <v>48.4</v>
+      </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74" s="3" t="s">
         <v>104</v>
       </c>
       <c r="B74" s="24" t="s">
-        <v>199</v>
-      </c>
-      <c r="C74" s="6"/>
-      <c r="D74" s="3"/>
+        <v>197</v>
+      </c>
+      <c r="C74" s="6">
+        <v>26.5</v>
+      </c>
+      <c r="D74" s="3">
+        <v>30.1</v>
+      </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75" s="3" t="s">
         <v>105</v>
       </c>
       <c r="B75" s="24" t="s">
-        <v>200</v>
-      </c>
-      <c r="C75" s="6"/>
-      <c r="D75" s="3"/>
+        <v>198</v>
+      </c>
+      <c r="C75" s="6">
+        <v>85.4</v>
+      </c>
+      <c r="D75" s="3">
+        <v>75.5</v>
+      </c>
     </row>
     <row r="76" spans="1:4">
       <c r="A76" s="1">
@@ -2073,7 +2433,9 @@
       <c r="B76" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="C76" s="6"/>
+      <c r="C76" s="6" t="s">
+        <v>264</v>
+      </c>
       <c r="D76" s="3"/>
     </row>
     <row r="77" spans="1:4">
@@ -2093,7 +2455,9 @@
       <c r="B78" s="6" t="s">
         <v>109</v>
       </c>
-      <c r="C78" s="6"/>
+      <c r="C78" s="6">
+        <v>92</v>
+      </c>
       <c r="D78" s="6"/>
     </row>
     <row r="79" spans="1:4">
@@ -2103,7 +2467,9 @@
       <c r="B79" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="C79" s="6"/>
+      <c r="C79" s="6">
+        <v>1</v>
+      </c>
       <c r="D79" s="6"/>
     </row>
     <row r="80" spans="1:4">
@@ -2113,7 +2479,9 @@
       <c r="B80" s="6" t="s">
         <v>113</v>
       </c>
-      <c r="C80" s="6"/>
+      <c r="C80" s="6">
+        <v>0</v>
+      </c>
       <c r="D80" s="6"/>
     </row>
     <row r="81" spans="1:4">
@@ -2123,7 +2491,9 @@
       <c r="B81" s="6" t="s">
         <v>115</v>
       </c>
-      <c r="C81" s="6"/>
+      <c r="C81" s="6">
+        <v>0</v>
+      </c>
       <c r="D81" s="6"/>
     </row>
     <row r="82" spans="1:4">
@@ -2133,7 +2503,9 @@
       <c r="B82" s="6" t="s">
         <v>117</v>
       </c>
-      <c r="C82" s="6"/>
+      <c r="C82" s="6">
+        <v>0</v>
+      </c>
       <c r="D82" s="6"/>
     </row>
     <row r="83" spans="1:4">
@@ -2143,7 +2515,9 @@
       <c r="B83" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="C83" s="6"/>
+      <c r="C83" s="6">
+        <v>7</v>
+      </c>
       <c r="D83" s="6"/>
     </row>
     <row r="84" spans="1:4">
@@ -2153,7 +2527,9 @@
       <c r="B84" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="C84" s="6"/>
+      <c r="C84" s="6">
+        <v>0</v>
+      </c>
       <c r="D84" s="6"/>
     </row>
     <row r="85" spans="1:4">
@@ -2163,7 +2539,9 @@
       <c r="B85" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C85" s="6"/>
+      <c r="C85" s="6">
+        <v>0.42</v>
+      </c>
       <c r="D85" s="3"/>
     </row>
     <row r="86" spans="1:4">
@@ -2193,8 +2571,12 @@
       <c r="B88" s="7" t="s">
         <v>125</v>
       </c>
-      <c r="C88" s="6"/>
-      <c r="D88" s="3"/>
+      <c r="C88" s="6">
+        <v>49.1</v>
+      </c>
+      <c r="D88" s="3">
+        <v>73.8</v>
+      </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89" s="1">
@@ -2203,8 +2585,12 @@
       <c r="B89" s="7" t="s">
         <v>126</v>
       </c>
-      <c r="C89" s="6"/>
-      <c r="D89" s="10"/>
+      <c r="C89" s="6">
+        <v>11.6</v>
+      </c>
+      <c r="D89" s="10">
+        <v>1.1000000000000001</v>
+      </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90" s="1">
@@ -2223,8 +2609,12 @@
       <c r="B91" s="7" t="s">
         <v>128</v>
       </c>
-      <c r="C91" s="6"/>
-      <c r="D91" s="10"/>
+      <c r="C91" s="6">
+        <v>74</v>
+      </c>
+      <c r="D91" s="10">
+        <v>70</v>
+      </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92" s="1"/>
@@ -2251,7 +2641,7 @@
         <v>9</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="95" spans="1:4">
@@ -2259,29 +2649,39 @@
         <v>9.1</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>202</v>
-      </c>
-      <c r="C95" s="9"/>
-      <c r="D95" s="10"/>
+        <v>200</v>
+      </c>
+      <c r="C95" s="10" t="s">
+        <v>251</v>
+      </c>
+      <c r="D95" s="10" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96" s="1">
         <v>9.1999999999999993</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>203</v>
-      </c>
-      <c r="C96" s="9"/>
-      <c r="D96" s="10"/>
+        <v>201</v>
+      </c>
+      <c r="C96" s="10" t="s">
+        <v>252</v>
+      </c>
+      <c r="D96" s="10" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97" s="1">
         <v>9.3000000000000007</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>204</v>
-      </c>
-      <c r="C97" s="9"/>
+        <v>202</v>
+      </c>
+      <c r="C97" s="10" t="s">
+        <v>253</v>
+      </c>
       <c r="D97" s="10"/>
     </row>
     <row r="98" spans="1:4">
@@ -2289,7 +2689,7 @@
         <v>10</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="99" spans="1:4">
@@ -2297,27 +2697,35 @@
         <v>10.1</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>206</v>
-      </c>
-      <c r="C99" s="9"/>
-      <c r="D99" s="10"/>
+        <v>204</v>
+      </c>
+      <c r="C99" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100" s="1">
         <v>10.199999999999999</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>207</v>
-      </c>
-      <c r="C100" s="9"/>
-      <c r="D100" s="10"/>
+        <v>205</v>
+      </c>
+      <c r="C100" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="D100" s="10" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="101" spans="1:4">
       <c r="A101" s="1">
         <v>10.3</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C101" s="9"/>
       <c r="D101" s="10"/>
@@ -2341,15 +2749,19 @@
         <v>82</v>
       </c>
     </row>
-    <row r="104" spans="1:4">
+    <row r="104" spans="1:4" ht="16.5">
       <c r="A104">
         <v>11.1</v>
       </c>
       <c r="B104" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="C104" s="9"/>
-      <c r="D104" s="9"/>
+      <c r="C104" s="27">
+        <v>11133</v>
+      </c>
+      <c r="D104" s="26">
+        <v>15.179399999999999</v>
+      </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105">
@@ -2358,8 +2770,12 @@
       <c r="B105" s="16" t="s">
         <v>135</v>
       </c>
-      <c r="C105" s="9"/>
-      <c r="D105" s="9"/>
+      <c r="C105" s="28">
+        <v>39633</v>
+      </c>
+      <c r="D105" s="26">
+        <v>39.782299999999999</v>
+      </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106">
@@ -2376,6 +2792,12 @@
       <c r="B107" s="16" t="s">
         <v>137</v>
       </c>
+      <c r="C107">
+        <v>920</v>
+      </c>
+      <c r="D107">
+        <v>60</v>
+      </c>
     </row>
     <row r="108" spans="1:4">
       <c r="A108">
@@ -2384,6 +2806,12 @@
       <c r="B108" s="16" t="s">
         <v>138</v>
       </c>
+      <c r="C108">
+        <v>2662</v>
+      </c>
+      <c r="D108">
+        <v>30018</v>
+      </c>
     </row>
     <row r="109" spans="1:4">
       <c r="B109" s="2" t="s">
@@ -2411,6 +2839,12 @@
       <c r="B111" s="16" t="s">
         <v>141</v>
       </c>
+      <c r="C111" t="s">
+        <v>267</v>
+      </c>
+      <c r="D111" t="s">
+        <v>267</v>
+      </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112">
@@ -2419,6 +2853,12 @@
       <c r="B112" s="16" t="s">
         <v>142</v>
       </c>
+      <c r="C112" t="s">
+        <v>266</v>
+      </c>
+      <c r="D112" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113">
@@ -2427,13 +2867,19 @@
       <c r="B113" s="16" t="s">
         <v>143</v>
       </c>
+      <c r="C113" t="s">
+        <v>268</v>
+      </c>
+      <c r="D113" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="114" spans="1:4">
       <c r="A114">
         <v>14</v>
       </c>
       <c r="B114" s="14" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -2443,6 +2889,12 @@
       <c r="B115" s="16" t="s">
         <v>144</v>
       </c>
+      <c r="C115" t="s">
+        <v>269</v>
+      </c>
+      <c r="D115" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116">
@@ -2451,6 +2903,12 @@
       <c r="B116" s="16" t="s">
         <v>145</v>
       </c>
+      <c r="C116" t="s">
+        <v>269</v>
+      </c>
+      <c r="D116" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117">
@@ -2459,6 +2917,12 @@
       <c r="B117" s="16" t="s">
         <v>146</v>
       </c>
+      <c r="C117" t="s">
+        <v>270</v>
+      </c>
+      <c r="D117" t="s">
+        <v>270</v>
+      </c>
     </row>
     <row r="118" spans="1:4">
       <c r="A118">
@@ -2467,6 +2931,12 @@
       <c r="B118" s="16" t="s">
         <v>147</v>
       </c>
+      <c r="C118" t="s">
+        <v>269</v>
+      </c>
+      <c r="D118" t="s">
+        <v>269</v>
+      </c>
     </row>
     <row r="119" spans="1:4">
       <c r="A119">
@@ -2626,6 +3096,9 @@
         <v>160</v>
       </c>
       <c r="C131" s="16"/>
+      <c r="D131" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="132" spans="1:4">
       <c r="A132">
@@ -2635,6 +3108,9 @@
         <v>161</v>
       </c>
       <c r="C132" s="16"/>
+      <c r="D132" t="s">
+        <v>294</v>
+      </c>
     </row>
     <row r="133" spans="1:4">
       <c r="A133">
@@ -2644,6 +3120,9 @@
         <v>162</v>
       </c>
       <c r="C133" s="16"/>
+      <c r="D133" t="s">
+        <v>295</v>
+      </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134">
@@ -2670,9 +3149,11 @@
       <c r="B136" s="16" t="s">
         <v>165</v>
       </c>
-      <c r="C136" s="16"/>
+      <c r="C136" s="16" t="s">
+        <v>292</v>
+      </c>
       <c r="D136" t="s">
-        <v>209</v>
+        <v>292</v>
       </c>
     </row>
     <row r="137" spans="1:4">
@@ -2718,7 +3199,12 @@
       <c r="B141" s="22" t="s">
         <v>170</v>
       </c>
-      <c r="C141" s="16"/>
+      <c r="C141" s="16">
+        <v>25</v>
+      </c>
+      <c r="D141">
+        <v>25</v>
+      </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142">
@@ -2727,7 +3213,12 @@
       <c r="B142" s="22" t="s">
         <v>171</v>
       </c>
-      <c r="C142" s="16"/>
+      <c r="C142" s="16">
+        <v>13</v>
+      </c>
+      <c r="D142">
+        <v>15</v>
+      </c>
     </row>
     <row r="143" spans="1:4">
       <c r="A143">
@@ -2736,7 +3227,14 @@
       <c r="B143" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="C143" s="16"/>
+      <c r="C143" s="16">
+        <f>AVERAGE(C141:C142)</f>
+        <v>19</v>
+      </c>
+      <c r="D143">
+        <f>AVERAGE(D141:D142)</f>
+        <v>20</v>
+      </c>
     </row>
     <row r="144" spans="1:4">
       <c r="A144">
@@ -2763,7 +3261,12 @@
       <c r="B146" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="C146" s="16"/>
+      <c r="C146" s="16">
+        <v>215</v>
+      </c>
+      <c r="D146">
+        <v>129</v>
+      </c>
     </row>
     <row r="147" spans="1:4">
       <c r="A147">
@@ -2772,32 +3275,47 @@
       <c r="B147" s="22" t="s">
         <v>176</v>
       </c>
-      <c r="C147" s="16"/>
+      <c r="C147" s="16">
+        <v>13</v>
+      </c>
+      <c r="D147">
+        <v>13</v>
+      </c>
     </row>
     <row r="148" spans="1:4">
       <c r="A148">
         <v>23</v>
       </c>
       <c r="B148" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="C148" s="16"/>
+        <v>297</v>
+      </c>
+      <c r="C148" s="16">
+        <v>7.2</v>
+      </c>
+      <c r="D148">
+        <v>7.3</v>
+      </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149">
         <v>24</v>
       </c>
       <c r="B149" t="s">
-        <v>178</v>
-      </c>
-      <c r="C149" s="16"/>
+        <v>296</v>
+      </c>
+      <c r="C149" s="16">
+        <v>8</v>
+      </c>
+      <c r="D149">
+        <v>13.6</v>
+      </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150">
         <v>25</v>
       </c>
       <c r="B150" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C150" s="16"/>
     </row>
@@ -2806,7 +3324,7 @@
         <v>26</v>
       </c>
       <c r="B151" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C151" s="16"/>
     </row>
@@ -2815,7 +3333,7 @@
         <v>26.1</v>
       </c>
       <c r="B152" s="22" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C152" s="16"/>
     </row>
@@ -2824,7 +3342,7 @@
         <v>26.2</v>
       </c>
       <c r="B153" s="22" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C153" s="16"/>
     </row>
@@ -2833,7 +3351,7 @@
         <v>26.3</v>
       </c>
       <c r="B154" s="22" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C154" s="16"/>
     </row>
@@ -2842,13 +3360,13 @@
         <v>26.4</v>
       </c>
       <c r="B155" s="22" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="C155" s="16"/>
     </row>
     <row r="156" spans="1:4">
       <c r="B156" s="2" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C156" s="5" t="s">
         <v>131</v>
@@ -2862,7 +3380,7 @@
         <v>27</v>
       </c>
       <c r="B157" s="15" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2870,16 +3388,27 @@
         <v>27.1</v>
       </c>
       <c r="B158" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="C158" s="16"/>
+        <v>211</v>
+      </c>
+      <c r="C158" t="s">
+        <v>272</v>
+      </c>
+      <c r="D158" t="s">
+        <v>271</v>
+      </c>
     </row>
     <row r="159" spans="1:4">
       <c r="A159">
         <v>27.2</v>
       </c>
       <c r="B159" s="22" t="s">
-        <v>215</v>
+        <v>212</v>
+      </c>
+      <c r="C159" t="s">
+        <v>273</v>
+      </c>
+      <c r="D159" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2887,267 +3416,350 @@
         <v>27.3</v>
       </c>
       <c r="B160" s="22" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="161" spans="1:3">
+        <v>213</v>
+      </c>
+      <c r="D160" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4">
       <c r="A161">
         <v>27.4</v>
       </c>
       <c r="B161" s="22" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="162" spans="1:3">
+        <v>214</v>
+      </c>
+      <c r="D161" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4">
       <c r="A162">
         <v>27.5</v>
       </c>
       <c r="B162" s="22" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="163" spans="1:3">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4">
       <c r="A163">
         <v>27.6</v>
       </c>
       <c r="B163" s="22" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="164" spans="1:4">
       <c r="A164">
         <v>27.7</v>
       </c>
       <c r="B164" s="22" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="165" spans="1:4">
       <c r="A165">
         <v>28</v>
       </c>
       <c r="B165" s="14" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="166" spans="1:4">
       <c r="A166">
         <v>28.1</v>
       </c>
       <c r="B166" s="22" t="s">
-        <v>221</v>
-      </c>
-      <c r="C166" s="16"/>
-    </row>
-    <row r="167" spans="1:3">
+        <v>218</v>
+      </c>
+      <c r="C166" t="s">
+        <v>288</v>
+      </c>
+      <c r="D166" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="167" spans="1:4">
       <c r="A167">
         <v>28.2</v>
       </c>
       <c r="B167" s="22" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3">
+        <v>219</v>
+      </c>
+      <c r="C167" t="s">
+        <v>291</v>
+      </c>
+      <c r="D167" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="168" spans="1:4">
       <c r="A168">
         <v>28.3</v>
       </c>
       <c r="B168" s="22" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3">
+        <v>220</v>
+      </c>
+      <c r="C168" t="s">
+        <v>290</v>
+      </c>
+      <c r="D168" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="169" spans="1:4">
       <c r="A169">
         <v>28.4</v>
       </c>
       <c r="B169" s="22" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3">
+        <v>221</v>
+      </c>
+      <c r="C169" t="s">
+        <v>289</v>
+      </c>
+      <c r="D169" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="170" spans="1:4">
       <c r="A170">
         <v>28.5</v>
       </c>
       <c r="B170" s="22" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="171" spans="1:4">
       <c r="A171">
         <v>28.6</v>
       </c>
       <c r="B171" s="22" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="172" spans="1:4">
       <c r="A172">
         <v>29</v>
       </c>
       <c r="B172" s="14" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="173" spans="1:4">
       <c r="A173">
         <v>29.1</v>
       </c>
       <c r="B173" s="22" t="s">
-        <v>227</v>
-      </c>
-      <c r="C173" s="16"/>
-    </row>
-    <row r="174" spans="1:3">
+        <v>224</v>
+      </c>
+      <c r="C173" s="16" t="s">
+        <v>284</v>
+      </c>
+      <c r="D173" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="174" spans="1:4">
       <c r="A174">
         <v>29.2</v>
       </c>
       <c r="B174" s="22" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3">
+        <v>225</v>
+      </c>
+      <c r="C174" t="s">
+        <v>285</v>
+      </c>
+      <c r="D174" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="175" spans="1:4">
       <c r="A175">
         <v>29.3</v>
       </c>
       <c r="B175" s="22" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3">
+        <v>226</v>
+      </c>
+      <c r="C175" t="s">
+        <v>286</v>
+      </c>
+      <c r="D175" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="176" spans="1:4">
       <c r="A176">
         <v>29.4</v>
       </c>
       <c r="B176" s="22" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3">
+        <v>227</v>
+      </c>
+      <c r="D176" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="177" spans="1:4">
       <c r="A177">
         <v>29.5</v>
       </c>
       <c r="B177" s="22" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3">
+        <v>228</v>
+      </c>
+      <c r="D177" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="178" spans="1:4">
       <c r="A178">
         <v>29.6</v>
       </c>
       <c r="B178" s="22" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3">
+        <v>229</v>
+      </c>
+      <c r="D178" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="179" spans="1:4">
       <c r="A179">
         <v>30</v>
       </c>
       <c r="B179" s="14" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="180" spans="1:3">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="180" spans="1:4">
       <c r="A180" s="16">
         <v>30.1</v>
       </c>
       <c r="B180" s="16" t="s">
-        <v>233</v>
-      </c>
-      <c r="C180" s="16"/>
-    </row>
-    <row r="181" spans="1:3">
+        <v>230</v>
+      </c>
+      <c r="C180" t="s">
+        <v>276</v>
+      </c>
+      <c r="D180" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="181" spans="1:4">
       <c r="A181" s="16">
         <v>30.2</v>
       </c>
       <c r="B181" s="16" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="182" spans="1:3">
+        <v>231</v>
+      </c>
+      <c r="C181" t="s">
+        <v>278</v>
+      </c>
+      <c r="D181" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="182" spans="1:4">
       <c r="A182" s="16">
         <v>30.3</v>
       </c>
       <c r="B182" s="16" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="183" spans="1:3">
+        <v>232</v>
+      </c>
+      <c r="D182" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="183" spans="1:4">
       <c r="A183" s="16">
         <v>30.4</v>
       </c>
       <c r="B183" s="16" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="184" spans="1:3">
+        <v>233</v>
+      </c>
+      <c r="D183" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="184" spans="1:4">
       <c r="A184" s="16">
         <v>30.5</v>
       </c>
       <c r="B184" s="16" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="185" spans="1:3">
+        <v>234</v>
+      </c>
+      <c r="D184" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="185" spans="1:4">
       <c r="A185" s="16">
         <v>30.6</v>
       </c>
       <c r="B185" s="16" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="186" spans="1:3">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="186" spans="1:4">
       <c r="A186">
         <v>31</v>
       </c>
       <c r="B186" s="14" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="187" spans="1:3">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="187" spans="1:4">
       <c r="A187" s="14">
         <v>31.1</v>
       </c>
       <c r="B187" s="16" t="s">
-        <v>239</v>
-      </c>
-      <c r="C187" s="16"/>
-    </row>
-    <row r="188" spans="1:3">
+        <v>236</v>
+      </c>
+      <c r="C187" s="16" t="s">
+        <v>279</v>
+      </c>
+      <c r="D187" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="188" spans="1:4">
       <c r="A188" s="14">
         <v>31.2</v>
       </c>
       <c r="B188" s="16" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="189" spans="1:3">
+        <v>237</v>
+      </c>
+      <c r="D188" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="189" spans="1:4">
       <c r="A189" s="14">
         <v>31.3</v>
       </c>
       <c r="B189" s="16" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="190" spans="1:3">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="190" spans="1:4">
       <c r="A190" s="14">
         <v>31.4</v>
       </c>
       <c r="B190" s="16" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="191" spans="1:3">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="191" spans="1:4">
       <c r="A191" s="14">
         <v>31.5</v>
       </c>
       <c r="B191" s="16" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="192" spans="1:3">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="192" spans="1:4">
       <c r="A192" s="14">
         <v>31.6</v>
       </c>
       <c r="B192" s="16" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3163,30 +3775,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B74:B75">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Valores Validos de entrada: &quot;Si&quot; o &quot;No&quot;_x000a_Si es que no se puede dejar en blanco_x000a__x000a_" sqref="C49:D55" xr:uid="{BAF48672-73FD-4231-93D4-13AD26F429C3}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Valores Validos de entrada: &quot;Si&quot; o &quot;No&quot;_x000a_Si es que no se puede dejar en blanco_x000a__x000a_" sqref="C49:D55">
       <formula1>"Si, No"</formula1>
     </dataValidation>
-    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Formato fecha" prompt="DD/MM/AAAA" sqref="D129" xr:uid="{0CC26212-6430-410E-8979-27DFBA36E156}">
+    <dataValidation type="date" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Formato fecha" prompt="DD/MM/AAAA" sqref="D129">
       <formula1>36526</formula1>
       <formula2>402133</formula2>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D136" xr:uid="{9ABE5371-2A2F-4500-B599-C42C1B3C7055}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D136">
       <formula1>"Af,Aw,Am"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D137" xr:uid="{1F3C7A60-42C1-4838-93A8-2D2A0D547E0F}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D137">
       <formula1>"Bsh,Bsk,Bhw,Bwk"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D138" xr:uid="{E3F7A7FB-B08A-48AB-A09E-BFCAACA262CC}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D138">
       <formula1>"Cdb,Cfc,Csa,Cfa,Cwa,Cwb"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D139" xr:uid="{5D300C50-C4CF-46DD-B628-47DF481CEA31}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D139">
       <formula1>"Dfa,Bwa,Dsa,Dfb,Dwb,Dsb"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C115:D118" xr:uid="{11A8FA3E-F4F7-43D9-84D4-67EC08F949B6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C115:D118">
       <formula1>"yes,no"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>